<commit_message>
Update network stats excel document
</commit_message>
<xml_diff>
--- a/project3/network_test_stats.xlsx
+++ b/project3/network_test_stats.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80a8a3a3b256c373/Studier 2015H/IT3105/project3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iver\OneDrive\Studier 2015H\IT3105\project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5796" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5796" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="200 rel" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>200 rel</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Results:</t>
   </si>
   <si>
-    <t>100 epochs</t>
-  </si>
-  <si>
     <t>time per epoch</t>
   </si>
   <si>
@@ -217,6 +214,27 @@
   </si>
   <si>
     <t>0.961</t>
+  </si>
+  <si>
+    <t>0.9873</t>
+  </si>
+  <si>
+    <t>0.9877</t>
+  </si>
+  <si>
+    <t>0.9875</t>
+  </si>
+  <si>
+    <t>0.9872</t>
+  </si>
+  <si>
+    <t>0.9878</t>
+  </si>
+  <si>
+    <t>0.9876</t>
+  </si>
+  <si>
+    <t>0.9882</t>
   </si>
 </sst>
 </file>
@@ -563,15 +581,15 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -579,10 +597,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -593,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>0.97919999999999996</v>
@@ -604,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -612,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -620,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -628,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -636,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -644,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -652,7 +670,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -660,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -668,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -676,7 +694,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -684,7 +702,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,7 +710,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
@@ -700,7 +718,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
@@ -708,7 +726,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
@@ -716,7 +734,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
@@ -724,7 +742,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -732,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
@@ -740,7 +758,7 @@
         <v>19</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
@@ -748,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -773,17 +791,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -792,13 +810,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -809,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -817,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -825,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -841,7 +859,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -857,7 +875,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -865,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -873,7 +891,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -881,7 +899,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,7 +915,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,7 +923,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
@@ -913,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
@@ -921,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
@@ -929,7 +947,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
@@ -937,7 +955,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -945,7 +963,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
@@ -953,7 +971,7 @@
         <v>19</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
@@ -961,7 +979,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -986,17 +1004,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -1005,10 +1023,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1019,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1027,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1035,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1051,7 +1069,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1059,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1067,7 +1085,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1075,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1083,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1091,7 +1109,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1099,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1107,7 +1125,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1115,7 +1133,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
@@ -1123,7 +1141,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
@@ -1131,7 +1149,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
@@ -1139,7 +1157,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
@@ -1147,7 +1165,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -1155,7 +1173,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
@@ -1163,7 +1181,7 @@
         <v>19</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
@@ -1171,7 +1189,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -1196,12 +1214,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -1210,10 +1228,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1224,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1232,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1240,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1256,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1264,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1272,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1280,7 +1298,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,7 +1306,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1296,7 +1314,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1304,7 +1322,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1320,7 +1338,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
@@ -1328,7 +1346,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
@@ -1336,7 +1354,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
@@ -1344,7 +1362,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
@@ -1352,7 +1370,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -1360,7 +1378,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
@@ -1368,7 +1386,7 @@
         <v>19</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
@@ -1376,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1387,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,191 +1419,192 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
       <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36">
-        <v>0.9849</v>
-      </c>
-      <c r="D36">
-        <v>0.98699999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B58">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B59">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B60">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B61">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B62">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B63">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B64">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65">
-        <v>30</v>
+      <c r="C55" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>